<commit_message>
first version with ROS pressure control (pressure-time trajectory) functionality
</commit_message>
<xml_diff>
--- a/msp_ws/jumpy/pin table.xlsx
+++ b/msp_ws/jumpy/pin table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="150">
   <si>
     <t xml:space="preserve">GPIO</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t xml:space="preserve">P1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debug pin</t>
   </si>
   <si>
     <t xml:space="preserve">P1.6</t>
@@ -1032,7 +1035,7 @@
   <dimension ref="A1:T87"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1378,8 +1381,12 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="6"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="10"/>
+      <c r="S9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="n">
@@ -1389,7 +1396,7 @@
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" s="12" t="n">
         <v>10</v>
@@ -1402,16 +1409,16 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="O10" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="O10" s="13" t="s">
-        <v>29</v>
       </c>
       <c r="P10" s="14" t="n">
         <v>10</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R10" s="6"/>
       <c r="S10" s="8"/>
@@ -1425,7 +1432,7 @@
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F11" s="12" t="n">
         <v>11</v>
@@ -1438,16 +1445,16 @@
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O11" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P11" s="14" t="n">
         <v>11</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R11" s="6"/>
       <c r="S11" s="8"/>
@@ -1461,7 +1468,7 @@
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F12" s="17" t="n">
         <v>16</v>
@@ -1482,7 +1489,7 @@
         <v>16</v>
       </c>
       <c r="T12" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,7 +1500,7 @@
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" s="17" t="n">
         <v>17</v>
@@ -1514,7 +1521,7 @@
         <v>16</v>
       </c>
       <c r="T13" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1525,7 +1532,7 @@
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F14" s="17" t="n">
         <v>18</v>
@@ -1534,16 +1541,16 @@
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
       <c r="J14" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="18" t="s">
         <v>38</v>
-      </c>
-      <c r="K14" s="18" t="s">
-        <v>37</v>
       </c>
       <c r="L14" s="18" t="n">
         <v>18</v>
       </c>
       <c r="M14" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N14" s="8"/>
       <c r="O14" s="9"/>
@@ -1554,7 +1561,7 @@
         <v>16</v>
       </c>
       <c r="T14" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1565,7 +1572,7 @@
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
       <c r="E15" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F15" s="17" t="n">
         <v>19</v>
@@ -1574,16 +1581,16 @@
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
       <c r="J15" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L15" s="18" t="n">
         <v>19</v>
       </c>
       <c r="M15" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N15" s="8"/>
       <c r="O15" s="9"/>
@@ -1601,16 +1608,16 @@
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F16" s="17" t="n">
         <v>20</v>
       </c>
       <c r="G16" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="13" t="s">
         <v>43</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>42</v>
       </c>
       <c r="I16" s="13" t="n">
         <v>20</v>
@@ -1635,16 +1642,16 @@
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F17" s="17" t="n">
         <v>21</v>
       </c>
       <c r="G17" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>44</v>
       </c>
       <c r="I17" s="13" t="n">
         <v>21</v>
@@ -1669,16 +1676,16 @@
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F18" s="17" t="n">
         <v>22</v>
       </c>
       <c r="G18" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="13" t="s">
         <v>47</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>46</v>
       </c>
       <c r="I18" s="13" t="n">
         <v>22</v>
@@ -1703,16 +1710,16 @@
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
       <c r="E19" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F19" s="17" t="n">
         <v>23</v>
       </c>
       <c r="G19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="13" t="s">
         <v>49</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>48</v>
       </c>
       <c r="I19" s="13" t="n">
         <v>23</v>
@@ -1737,7 +1744,7 @@
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F20" s="21" t="n">
         <v>32</v>
@@ -1765,7 +1772,7 @@
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F21" s="21" t="n">
         <v>33</v>
@@ -1793,7 +1800,7 @@
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F22" s="21" t="n">
         <v>34</v>
@@ -1802,16 +1809,16 @@
       <c r="H22" s="0"/>
       <c r="I22" s="0"/>
       <c r="J22" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K22" s="22" t="s">
         <v>53</v>
-      </c>
-      <c r="K22" s="22" t="s">
-        <v>52</v>
       </c>
       <c r="L22" s="22" t="n">
         <v>34</v>
       </c>
       <c r="M22" s="22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N22" s="8"/>
       <c r="O22" s="9"/>
@@ -1822,7 +1829,7 @@
         <v>16</v>
       </c>
       <c r="T22" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1833,7 +1840,7 @@
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F23" s="21" t="n">
         <v>35</v>
@@ -1842,16 +1849,16 @@
       <c r="H23" s="0"/>
       <c r="I23" s="0"/>
       <c r="J23" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K23" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L23" s="22" t="n">
         <v>35</v>
       </c>
       <c r="M23" s="22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N23" s="8"/>
       <c r="O23" s="9"/>
@@ -1862,7 +1869,7 @@
         <v>16</v>
       </c>
       <c r="T23" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1873,7 +1880,7 @@
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
       <c r="E24" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F24" s="21" t="n">
         <v>36</v>
@@ -1901,7 +1908,7 @@
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F25" s="21" t="n">
         <v>37</v>
@@ -1922,7 +1929,7 @@
         <v>16</v>
       </c>
       <c r="T25" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1933,7 +1940,7 @@
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F26" s="21" t="n">
         <v>38</v>
@@ -1946,23 +1953,23 @@
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="O26" s="22" t="s">
         <v>61</v>
-      </c>
-      <c r="O26" s="22" t="s">
-        <v>60</v>
       </c>
       <c r="P26" s="22" t="n">
         <v>38</v>
       </c>
       <c r="Q26" s="21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R26" s="6"/>
       <c r="S26" s="8" t="s">
         <v>16</v>
       </c>
       <c r="T26" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1973,7 +1980,7 @@
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F27" s="21" t="n">
         <v>39</v>
@@ -1986,20 +1993,24 @@
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
       <c r="N27" s="20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O27" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P27" s="22" t="n">
         <v>39</v>
       </c>
       <c r="Q27" s="21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R27" s="6"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="10"/>
+      <c r="S27" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="T27" s="10" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="23" t="n">
@@ -2009,13 +2020,13 @@
         <v>13</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D28" s="17" t="n">
         <v>56</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F28" s="25" t="n">
         <v>56</v>
@@ -2043,13 +2054,13 @@
         <v>12</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D29" s="17" t="n">
         <v>57</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F29" s="25" t="n">
         <v>57</v>
@@ -2077,13 +2088,13 @@
         <v>11</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D30" s="17" t="n">
         <v>58</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F30" s="25" t="n">
         <v>58</v>
@@ -2111,13 +2122,13 @@
         <v>10</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D31" s="17" t="n">
         <v>59</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F31" s="25" t="n">
         <v>59</v>
@@ -2145,13 +2156,13 @@
         <v>9</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D32" s="17" t="n">
         <v>60</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F32" s="25" t="n">
         <v>60</v>
@@ -2172,7 +2183,7 @@
         <v>16</v>
       </c>
       <c r="T32" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2183,13 +2194,13 @@
         <v>8</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D33" s="17" t="n">
         <v>61</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F33" s="25" t="n">
         <v>61</v>
@@ -2210,7 +2221,7 @@
         <v>16</v>
       </c>
       <c r="T33" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2221,13 +2232,13 @@
         <v>7</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D34" s="17" t="n">
         <v>62</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F34" s="25" t="n">
         <v>62</v>
@@ -2248,7 +2259,7 @@
         <v>16</v>
       </c>
       <c r="T34" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2259,13 +2270,13 @@
         <v>6</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D35" s="17" t="n">
         <v>63</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F35" s="25" t="n">
         <v>63</v>
@@ -2286,7 +2297,7 @@
         <v>16</v>
       </c>
       <c r="T35" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,13 +2308,13 @@
         <v>5</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D36" s="12" t="n">
         <v>64</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F36" s="28" t="n">
         <v>64</v>
@@ -2324,7 +2335,7 @@
         <v>16</v>
       </c>
       <c r="T36" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2335,13 +2346,13 @@
         <v>4</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D37" s="12" t="n">
         <v>65</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F37" s="28" t="n">
         <v>65</v>
@@ -2362,7 +2373,7 @@
         <v>16</v>
       </c>
       <c r="T37" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2373,13 +2384,13 @@
         <v>3</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D38" s="12" t="n">
         <v>66</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F38" s="28" t="n">
         <v>66</v>
@@ -2400,7 +2411,7 @@
         <v>16</v>
       </c>
       <c r="T38" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2411,13 +2422,13 @@
         <v>2</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D39" s="12" t="n">
         <v>67</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F39" s="28" t="n">
         <v>67</v>
@@ -2445,13 +2456,13 @@
         <v>1</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D40" s="12" t="n">
         <v>68</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F40" s="28" t="n">
         <v>68</v>
@@ -2472,7 +2483,7 @@
         <v>16</v>
       </c>
       <c r="T40" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2483,13 +2494,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D41" s="12" t="n">
         <v>69</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F41" s="28" t="n">
         <v>69</v>
@@ -2510,7 +2521,7 @@
         <v>16</v>
       </c>
       <c r="T41" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2521,16 +2532,16 @@
       <c r="C42" s="9"/>
       <c r="D42" s="10"/>
       <c r="E42" s="27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F42" s="28" t="n">
         <v>70</v>
       </c>
       <c r="G42" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="H42" s="22" t="s">
         <v>88</v>
-      </c>
-      <c r="H42" s="22" t="s">
-        <v>87</v>
       </c>
       <c r="I42" s="22" t="n">
         <v>70</v>
@@ -2555,16 +2566,16 @@
       <c r="C43" s="9"/>
       <c r="D43" s="10"/>
       <c r="E43" s="27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F43" s="28" t="n">
         <v>71</v>
       </c>
       <c r="G43" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H43" s="22" t="s">
         <v>90</v>
-      </c>
-      <c r="H43" s="22" t="s">
-        <v>89</v>
       </c>
       <c r="I43" s="22" t="n">
         <v>71</v>
@@ -2589,13 +2600,13 @@
         <v>15</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D44" s="21" t="n">
         <v>54</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F44" s="31" t="n">
         <v>54</v>
@@ -2623,13 +2634,13 @@
         <v>14</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D45" s="21" t="n">
         <v>55</v>
       </c>
       <c r="E45" s="30" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F45" s="31" t="n">
         <v>55</v>
@@ -2657,7 +2668,7 @@
       <c r="C46" s="9"/>
       <c r="D46" s="10"/>
       <c r="E46" s="30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F46" s="31" t="n">
         <v>76</v>
@@ -2685,7 +2696,7 @@
       <c r="C47" s="9"/>
       <c r="D47" s="10"/>
       <c r="E47" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F47" s="31" t="n">
         <v>77</v>
@@ -2713,7 +2724,7 @@
       <c r="C48" s="9"/>
       <c r="D48" s="10"/>
       <c r="E48" s="30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F48" s="31" t="n">
         <v>78</v>
@@ -2726,23 +2737,23 @@
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
       <c r="N48" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="O48" s="18" t="s">
         <v>96</v>
-      </c>
-      <c r="O48" s="18" t="s">
-        <v>95</v>
       </c>
       <c r="P48" s="32" t="n">
         <v>78</v>
       </c>
       <c r="Q48" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R48" s="6"/>
       <c r="S48" s="8" t="s">
         <v>16</v>
       </c>
       <c r="T48" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2753,7 +2764,7 @@
       <c r="C49" s="9"/>
       <c r="D49" s="10"/>
       <c r="E49" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F49" s="31" t="n">
         <v>79</v>
@@ -2766,23 +2777,23 @@
       <c r="L49" s="9"/>
       <c r="M49" s="9"/>
       <c r="N49" s="16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O49" s="18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P49" s="32" t="n">
         <v>79</v>
       </c>
       <c r="Q49" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R49" s="6"/>
       <c r="S49" s="8" t="s">
         <v>16</v>
       </c>
       <c r="T49" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2793,16 +2804,16 @@
       <c r="C50" s="9"/>
       <c r="D50" s="10"/>
       <c r="E50" s="30" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F50" s="31" t="n">
         <v>80</v>
       </c>
       <c r="G50" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="H50" s="22" t="s">
         <v>101</v>
-      </c>
-      <c r="H50" s="22" t="s">
-        <v>100</v>
       </c>
       <c r="I50" s="22" t="n">
         <v>80</v>
@@ -2812,23 +2823,23 @@
       <c r="L50" s="9"/>
       <c r="M50" s="9"/>
       <c r="N50" s="24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O50" s="33" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P50" s="34" t="n">
         <v>80</v>
       </c>
       <c r="Q50" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R50" s="6"/>
       <c r="S50" s="8" t="s">
         <v>16</v>
       </c>
       <c r="T50" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2839,16 +2850,16 @@
       <c r="C51" s="9"/>
       <c r="D51" s="10"/>
       <c r="E51" s="30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F51" s="31" t="n">
         <v>81</v>
       </c>
       <c r="G51" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="H51" s="22" t="s">
         <v>105</v>
-      </c>
-      <c r="H51" s="22" t="s">
-        <v>104</v>
       </c>
       <c r="I51" s="22" t="n">
         <v>81</v>
@@ -2858,23 +2869,23 @@
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
       <c r="N51" s="24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O51" s="33" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="P51" s="34" t="n">
         <v>81</v>
       </c>
       <c r="Q51" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R51" s="6"/>
       <c r="S51" s="8" t="s">
         <v>16</v>
       </c>
       <c r="T51" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2959,10 +2970,10 @@
       <c r="E55" s="8"/>
       <c r="F55" s="10"/>
       <c r="G55" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I55" s="13" t="n">
         <v>91</v>
@@ -2989,10 +3000,10 @@
       <c r="E56" s="8"/>
       <c r="F56" s="10"/>
       <c r="G56" s="18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I56" s="18" t="n">
         <v>26</v>
@@ -3019,10 +3030,10 @@
       <c r="E57" s="8"/>
       <c r="F57" s="10"/>
       <c r="G57" s="18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H57" s="18" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I57" s="18" t="n">
         <v>27</v>
@@ -3049,10 +3060,10 @@
       <c r="E58" s="8"/>
       <c r="F58" s="10"/>
       <c r="G58" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H58" s="18" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I58" s="18" t="n">
         <v>28</v>
@@ -3079,10 +3090,10 @@
       <c r="E59" s="8"/>
       <c r="F59" s="10"/>
       <c r="G59" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H59" s="18" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I59" s="18" t="n">
         <v>29</v>
@@ -3109,10 +3120,10 @@
       <c r="E60" s="8"/>
       <c r="F60" s="10"/>
       <c r="G60" s="18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H60" s="18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I60" s="18" t="n">
         <v>30</v>
@@ -3139,10 +3150,10 @@
       <c r="E61" s="8"/>
       <c r="F61" s="10"/>
       <c r="G61" s="22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H61" s="22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I61" s="22" t="n">
         <v>31</v>
@@ -3167,7 +3178,7 @@
         <v>23</v>
       </c>
       <c r="C62" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D62" s="28" t="n">
         <v>46</v>
@@ -3175,10 +3186,10 @@
       <c r="E62" s="8"/>
       <c r="F62" s="10"/>
       <c r="G62" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="H62" s="33" t="s">
         <v>122</v>
-      </c>
-      <c r="H62" s="33" t="s">
-        <v>121</v>
       </c>
       <c r="I62" s="33" t="n">
         <v>46</v>
@@ -3203,7 +3214,7 @@
         <v>22</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D63" s="28" t="n">
         <v>47</v>
@@ -3233,7 +3244,7 @@
         <v>21</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D64" s="28" t="n">
         <v>48</v>
@@ -3263,7 +3274,7 @@
         <v>20</v>
       </c>
       <c r="C65" s="37" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D65" s="28" t="n">
         <v>49</v>
@@ -3293,7 +3304,7 @@
         <v>19</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D66" s="28" t="n">
         <v>50</v>
@@ -3323,7 +3334,7 @@
         <v>18</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D67" s="28" t="n">
         <v>51</v>
@@ -3353,7 +3364,7 @@
         <v>17</v>
       </c>
       <c r="C68" s="33" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D68" s="25" t="n">
         <v>52</v>
@@ -3383,7 +3394,7 @@
         <v>16</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D69" s="25" t="n">
         <v>53</v>
@@ -3415,10 +3426,10 @@
       <c r="E70" s="8"/>
       <c r="F70" s="10"/>
       <c r="G70" s="33" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H70" s="33" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I70" s="33" t="n">
         <v>74</v>
@@ -3445,10 +3456,10 @@
       <c r="E71" s="8"/>
       <c r="F71" s="10"/>
       <c r="G71" s="33" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H71" s="33" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I71" s="33" t="n">
         <v>75</v>
@@ -3526,16 +3537,16 @@
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
       <c r="J74" s="24" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K74" s="33" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L74" s="33" t="n">
         <v>98</v>
       </c>
       <c r="M74" s="33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N74" s="8"/>
       <c r="O74" s="9"/>
@@ -3558,16 +3569,16 @@
       <c r="H75" s="9"/>
       <c r="I75" s="9"/>
       <c r="J75" s="24" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K75" s="33" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L75" s="33" t="n">
         <v>99</v>
       </c>
       <c r="M75" s="33" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N75" s="8"/>
       <c r="O75" s="9"/>
@@ -3642,16 +3653,16 @@
       <c r="L78" s="9"/>
       <c r="M78" s="9"/>
       <c r="N78" s="24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O78" s="33" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="P78" s="34" t="n">
         <v>2</v>
       </c>
       <c r="Q78" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R78" s="6"/>
       <c r="S78" s="8"/>
@@ -3674,16 +3685,16 @@
       <c r="L79" s="9"/>
       <c r="M79" s="9"/>
       <c r="N79" s="24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O79" s="33" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="P79" s="34" t="n">
         <v>3</v>
       </c>
       <c r="Q79" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R79" s="6"/>
       <c r="S79" s="8"/>
@@ -3699,10 +3710,10 @@
       <c r="E80" s="8"/>
       <c r="F80" s="10"/>
       <c r="G80" s="24" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H80" s="33" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I80" s="33" t="n">
         <v>24</v>
@@ -3729,10 +3740,10 @@
       <c r="E81" s="8"/>
       <c r="F81" s="10"/>
       <c r="G81" s="33" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H81" s="33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I81" s="33" t="n">
         <v>25</v>
@@ -3751,7 +3762,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="40" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B82" s="8"/>
       <c r="C82" s="9"/>
@@ -3775,7 +3786,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="40" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B83" s="8"/>
       <c r="C83" s="9"/>
@@ -3799,7 +3810,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="40" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="9"/>
@@ -3823,7 +3834,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="40" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B85" s="8"/>
       <c r="C85" s="9"/>
@@ -3847,7 +3858,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="40" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B86" s="8"/>
       <c r="C86" s="9"/>
@@ -3871,7 +3882,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="41" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B87" s="42"/>
       <c r="C87" s="43"/>

</xml_diff>

<commit_message>
updated to reflect MSP wiring
</commit_message>
<xml_diff>
--- a/msp_ws/jumpy/pin table.xlsx
+++ b/msp_ws/jumpy/pin table.xlsx
@@ -15,6 +15,13 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$3:$T$87</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$3:$T$87</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$3:$T$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$3:$T$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$3:$T$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$3:$T$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$3:$T$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$3:$T$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$3:$T$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$3:$T$87</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="147">
   <si>
     <t xml:space="preserve">GPIO</t>
   </si>
@@ -157,6 +164,9 @@
     <t xml:space="preserve">TDX</t>
   </si>
   <si>
+    <t xml:space="preserve">external LED</t>
+  </si>
+  <si>
     <t xml:space="preserve">P2.4</t>
   </si>
   <si>
@@ -196,13 +206,13 @@
     <t xml:space="preserve">A2</t>
   </si>
   <si>
-    <t xml:space="preserve">Valve 1, inf</t>
+    <t xml:space="preserve">valve, knee R inf</t>
   </si>
   <si>
     <t xml:space="preserve">P3.3</t>
   </si>
   <si>
-    <t xml:space="preserve">Valve 1, vent</t>
+    <t xml:space="preserve">valve, knee R def</t>
   </si>
   <si>
     <t xml:space="preserve">P3.4</t>
@@ -211,7 +221,7 @@
     <t xml:space="preserve">P3.5</t>
   </si>
   <si>
-    <t xml:space="preserve">Valve 2, inf</t>
+    <t xml:space="preserve">valve, hip R inf</t>
   </si>
   <si>
     <t xml:space="preserve">P3.6</t>
@@ -220,7 +230,7 @@
     <t xml:space="preserve">B2</t>
   </si>
   <si>
-    <t xml:space="preserve">Valve 2, vent</t>
+    <t xml:space="preserve">valve, hip R def</t>
   </si>
   <si>
     <t xml:space="preserve">P3.7</t>
@@ -241,49 +251,37 @@
     <t xml:space="preserve">P4.4</t>
   </si>
   <si>
-    <t xml:space="preserve">encoder, joint 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">P4.5</t>
   </si>
   <si>
-    <t xml:space="preserve">encoder, joint 3</t>
-  </si>
-  <si>
     <t xml:space="preserve">P4.6</t>
   </si>
   <si>
-    <t xml:space="preserve">encoder, joint 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">P4.7</t>
   </si>
   <si>
-    <t xml:space="preserve">encoder, joint 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">P5.0</t>
   </si>
   <si>
-    <t xml:space="preserve">pres trans, act 4 (K,L)</t>
+    <t xml:space="preserve">pres trans, knee L</t>
   </si>
   <si>
     <t xml:space="preserve">P5.1</t>
   </si>
   <si>
-    <t xml:space="preserve">pres trans, act 3 (H,L)</t>
+    <t xml:space="preserve">pres trans, hip L</t>
   </si>
   <si>
     <t xml:space="preserve">P5.2</t>
   </si>
   <si>
-    <t xml:space="preserve">pres trans, act 2 (H,R)</t>
+    <t xml:space="preserve">pres trans, hip R</t>
   </si>
   <si>
     <t xml:space="preserve">P5.3</t>
   </si>
   <si>
-    <t xml:space="preserve">pres trans, act 1 (K,R)</t>
+    <t xml:space="preserve">pres trans, knee R</t>
   </si>
   <si>
     <t xml:space="preserve">P5.4</t>
@@ -310,9 +308,15 @@
     <t xml:space="preserve">P6.0</t>
   </si>
   <si>
+    <t xml:space="preserve">encoder 1 ch A</t>
+  </si>
+  <si>
     <t xml:space="preserve">P6.1</t>
   </si>
   <si>
+    <t xml:space="preserve">encoder 1 ch B</t>
+  </si>
+  <si>
     <t xml:space="preserve">P6.2</t>
   </si>
   <si>
@@ -325,15 +329,12 @@
     <t xml:space="preserve">B1</t>
   </si>
   <si>
-    <t xml:space="preserve">Valve 3, inf</t>
+    <t xml:space="preserve">encoder 1 ch X</t>
   </si>
   <si>
     <t xml:space="preserve">P6.5</t>
   </si>
   <si>
-    <t xml:space="preserve">Valve 3, vent</t>
-  </si>
-  <si>
     <t xml:space="preserve">P6.6</t>
   </si>
   <si>
@@ -343,16 +344,10 @@
     <t xml:space="preserve">B3</t>
   </si>
   <si>
-    <t xml:space="preserve">Valve 4, inf</t>
-  </si>
-  <si>
     <t xml:space="preserve">P6.7</t>
   </si>
   <si>
     <t xml:space="preserve">TA2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valve 4, vent</t>
   </si>
   <si>
     <t xml:space="preserve">TA0.0</t>
@@ -958,9 +953,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>312480</xdr:colOff>
+      <xdr:colOff>309960</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>173880</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -974,8 +969,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="26288280" y="4881960"/>
-          <a:ext cx="5484960" cy="2873520"/>
+          <a:off x="26688240" y="4881960"/>
+          <a:ext cx="5482800" cy="2871000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -996,9 +991,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>338760</xdr:colOff>
+      <xdr:colOff>336240</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1012,8 +1007,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="31761360" y="4723560"/>
-          <a:ext cx="6515280" cy="2842920"/>
+          <a:off x="32161680" y="4723560"/>
+          <a:ext cx="6512400" cy="2840400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1036,30 +1031,24 @@
   <dimension ref="A1:T87"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T27" activeCellId="0" sqref="T27"/>
+      <selection pane="topLeft" activeCell="O44" activeCellId="0" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="19" min="18" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1585,8 +1574,12 @@
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
       <c r="Q15" s="9"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="9"/>
+      <c r="S15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="T15" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="n">
@@ -1596,16 +1589,16 @@
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
       <c r="E16" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F16" s="16" t="n">
         <v>20</v>
       </c>
       <c r="G16" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>43</v>
       </c>
       <c r="I16" s="12" t="n">
         <v>20</v>
@@ -1629,16 +1622,16 @@
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
       <c r="E17" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F17" s="16" t="n">
         <v>21</v>
       </c>
       <c r="G17" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="I17" s="12" t="n">
         <v>21</v>
@@ -1662,16 +1655,16 @@
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
       <c r="E18" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F18" s="16" t="n">
         <v>22</v>
       </c>
       <c r="G18" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="I18" s="12" t="n">
         <v>22</v>
@@ -1695,16 +1688,16 @@
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
       <c r="E19" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F19" s="16" t="n">
         <v>23</v>
       </c>
       <c r="G19" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="I19" s="12" t="n">
         <v>23</v>
@@ -1728,7 +1721,7 @@
       <c r="C20" s="8"/>
       <c r="D20" s="9"/>
       <c r="E20" s="19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F20" s="20" t="n">
         <v>32</v>
@@ -1755,7 +1748,7 @@
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
       <c r="E21" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F21" s="20" t="n">
         <v>33</v>
@@ -1773,7 +1766,7 @@
       <c r="Q21" s="9"/>
       <c r="S21" s="7"/>
       <c r="T21" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,7 +1777,7 @@
       <c r="C22" s="8"/>
       <c r="D22" s="9"/>
       <c r="E22" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F22" s="20" t="n">
         <v>34</v>
@@ -1793,10 +1786,10 @@
       <c r="H22" s="0"/>
       <c r="I22" s="0"/>
       <c r="J22" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22" s="21" t="s">
         <v>55</v>
-      </c>
-      <c r="K22" s="21" t="s">
-        <v>54</v>
       </c>
       <c r="L22" s="21" t="n">
         <v>34</v>
@@ -1812,7 +1805,7 @@
         <v>16</v>
       </c>
       <c r="T22" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1823,7 +1816,7 @@
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
       <c r="E23" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F23" s="20" t="n">
         <v>35</v>
@@ -1832,10 +1825,10 @@
       <c r="H23" s="0"/>
       <c r="I23" s="0"/>
       <c r="J23" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K23" s="21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L23" s="21" t="n">
         <v>35</v>
@@ -1851,7 +1844,7 @@
         <v>16</v>
       </c>
       <c r="T23" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,7 +1855,7 @@
       <c r="C24" s="8"/>
       <c r="D24" s="9"/>
       <c r="E24" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F24" s="20" t="n">
         <v>36</v>
@@ -1889,7 +1882,7 @@
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
       <c r="E25" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F25" s="20" t="n">
         <v>37</v>
@@ -1909,7 +1902,7 @@
         <v>16</v>
       </c>
       <c r="T25" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1920,7 +1913,7 @@
       <c r="C26" s="8"/>
       <c r="D26" s="9"/>
       <c r="E26" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F26" s="20" t="n">
         <v>38</v>
@@ -1933,10 +1926,10 @@
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
       <c r="N26" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="O26" s="21" t="s">
         <v>63</v>
-      </c>
-      <c r="O26" s="21" t="s">
-        <v>62</v>
       </c>
       <c r="P26" s="21" t="n">
         <v>38</v>
@@ -1948,7 +1941,7 @@
         <v>16</v>
       </c>
       <c r="T26" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1959,7 +1952,7 @@
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F27" s="20" t="n">
         <v>39</v>
@@ -1972,10 +1965,10 @@
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
       <c r="N27" s="19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O27" s="21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P27" s="21" t="n">
         <v>39</v>
@@ -1998,13 +1991,13 @@
         <v>13</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D28" s="16" t="n">
         <v>56</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F28" s="24" t="n">
         <v>56</v>
@@ -2031,13 +2024,13 @@
         <v>12</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D29" s="16" t="n">
         <v>57</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F29" s="24" t="n">
         <v>57</v>
@@ -2064,13 +2057,13 @@
         <v>11</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D30" s="16" t="n">
         <v>58</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F30" s="24" t="n">
         <v>58</v>
@@ -2097,13 +2090,13 @@
         <v>10</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D31" s="16" t="n">
         <v>59</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F31" s="24" t="n">
         <v>59</v>
@@ -2130,13 +2123,13 @@
         <v>9</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D32" s="16" t="n">
         <v>60</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F32" s="24" t="n">
         <v>60</v>
@@ -2152,12 +2145,8 @@
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
       <c r="Q32" s="9"/>
-      <c r="S32" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T32" s="9" t="s">
-        <v>71</v>
-      </c>
+      <c r="S32" s="7"/>
+      <c r="T32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="n">
@@ -2193,7 +2182,7 @@
         <v>16</v>
       </c>
       <c r="T33" s="9" t="s">
-        <v>73</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2204,13 +2193,13 @@
         <v>7</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D34" s="16" t="n">
         <v>62</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F34" s="24" t="n">
         <v>62</v>
@@ -2230,7 +2219,7 @@
         <v>16</v>
       </c>
       <c r="T34" s="9" t="s">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2241,13 +2230,13 @@
         <v>6</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D35" s="16" t="n">
         <v>63</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F35" s="24" t="n">
         <v>63</v>
@@ -2267,7 +2256,7 @@
         <v>16</v>
       </c>
       <c r="T35" s="9" t="s">
-        <v>77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2278,13 +2267,13 @@
         <v>5</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D36" s="11" t="n">
         <v>64</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F36" s="27" t="n">
         <v>64</v>
@@ -2304,7 +2293,7 @@
         <v>16</v>
       </c>
       <c r="T36" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2315,13 +2304,13 @@
         <v>4</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D37" s="11" t="n">
         <v>65</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F37" s="27" t="n">
         <v>65</v>
@@ -2341,7 +2330,7 @@
         <v>16</v>
       </c>
       <c r="T37" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2352,13 +2341,13 @@
         <v>3</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D38" s="11" t="n">
         <v>66</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F38" s="27" t="n">
         <v>66</v>
@@ -2378,7 +2367,7 @@
         <v>16</v>
       </c>
       <c r="T38" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2389,13 +2378,13 @@
         <v>2</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D39" s="11" t="n">
         <v>67</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F39" s="27" t="n">
         <v>67</v>
@@ -2415,7 +2404,7 @@
         <v>16</v>
       </c>
       <c r="T39" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2426,13 +2415,13 @@
         <v>1</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D40" s="11" t="n">
         <v>68</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F40" s="27" t="n">
         <v>68</v>
@@ -2459,13 +2448,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D41" s="11" t="n">
         <v>69</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F41" s="27" t="n">
         <v>69</v>
@@ -2485,7 +2474,7 @@
         <v>16</v>
       </c>
       <c r="T41" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,16 +2485,16 @@
       <c r="C42" s="8"/>
       <c r="D42" s="9"/>
       <c r="E42" s="26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F42" s="27" t="n">
         <v>70</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I42" s="21" t="n">
         <v>70</v>
@@ -2529,16 +2518,16 @@
       <c r="C43" s="8"/>
       <c r="D43" s="9"/>
       <c r="E43" s="26" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F43" s="27" t="n">
         <v>71</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I43" s="21" t="n">
         <v>71</v>
@@ -2562,13 +2551,13 @@
         <v>15</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D44" s="20" t="n">
         <v>54</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F44" s="30" t="n">
         <v>54</v>
@@ -2585,7 +2574,9 @@
       <c r="P44" s="8"/>
       <c r="Q44" s="9"/>
       <c r="S44" s="7"/>
-      <c r="T44" s="9"/>
+      <c r="T44" s="9" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="28" t="n">
@@ -2595,13 +2586,13 @@
         <v>14</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D45" s="20" t="n">
         <v>55</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F45" s="30" t="n">
         <v>55</v>
@@ -2618,7 +2609,9 @@
       <c r="P45" s="8"/>
       <c r="Q45" s="9"/>
       <c r="S45" s="7"/>
-      <c r="T45" s="9"/>
+      <c r="T45" s="9" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="28" t="n">
@@ -2628,7 +2621,7 @@
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
       <c r="E46" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F46" s="30" t="n">
         <v>76</v>
@@ -2655,7 +2648,7 @@
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F47" s="30" t="n">
         <v>77</v>
@@ -2682,7 +2675,7 @@
       <c r="C48" s="8"/>
       <c r="D48" s="9"/>
       <c r="E48" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F48" s="30" t="n">
         <v>78</v>
@@ -2695,10 +2688,10 @@
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
       <c r="N48" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O48" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P48" s="31" t="n">
         <v>78</v>
@@ -2706,11 +2699,9 @@
       <c r="Q48" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="S48" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="S48" s="7"/>
       <c r="T48" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2721,7 +2712,7 @@
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F49" s="30" t="n">
         <v>79</v>
@@ -2734,10 +2725,10 @@
       <c r="L49" s="8"/>
       <c r="M49" s="8"/>
       <c r="N49" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O49" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P49" s="31" t="n">
         <v>79</v>
@@ -2745,12 +2736,8 @@
       <c r="Q49" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="S49" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T49" s="9" t="s">
-        <v>101</v>
-      </c>
+      <c r="S49" s="7"/>
+      <c r="T49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="28" t="n">
@@ -2760,16 +2747,16 @@
       <c r="C50" s="8"/>
       <c r="D50" s="9"/>
       <c r="E50" s="29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F50" s="30" t="n">
         <v>80</v>
       </c>
       <c r="G50" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I50" s="21" t="n">
         <v>80</v>
@@ -2779,10 +2766,10 @@
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
       <c r="N50" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O50" s="32" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="P50" s="33" t="n">
         <v>80</v>
@@ -2790,12 +2777,8 @@
       <c r="Q50" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="S50" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T50" s="9" t="s">
-        <v>105</v>
-      </c>
+      <c r="S50" s="7"/>
+      <c r="T50" s="9"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="28" t="n">
@@ -2805,16 +2788,16 @@
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F51" s="30" t="n">
         <v>81</v>
       </c>
       <c r="G51" s="19" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H51" s="21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I51" s="21" t="n">
         <v>81</v>
@@ -2824,10 +2807,10 @@
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
       <c r="N51" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O51" s="32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="P51" s="33" t="n">
         <v>81</v>
@@ -2835,12 +2818,8 @@
       <c r="Q51" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="S51" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T51" s="9" t="s">
-        <v>108</v>
-      </c>
+      <c r="S51" s="7"/>
+      <c r="T51" s="9"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="34" t="n">
@@ -2921,10 +2900,10 @@
       <c r="E55" s="7"/>
       <c r="F55" s="9"/>
       <c r="G55" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I55" s="12" t="n">
         <v>91</v>
@@ -2950,10 +2929,10 @@
       <c r="E56" s="7"/>
       <c r="F56" s="9"/>
       <c r="G56" s="17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I56" s="17" t="n">
         <v>26</v>
@@ -2979,10 +2958,10 @@
       <c r="E57" s="7"/>
       <c r="F57" s="9"/>
       <c r="G57" s="17" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I57" s="17" t="n">
         <v>27</v>
@@ -3008,10 +2987,10 @@
       <c r="E58" s="7"/>
       <c r="F58" s="9"/>
       <c r="G58" s="17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I58" s="17" t="n">
         <v>28</v>
@@ -3037,10 +3016,10 @@
       <c r="E59" s="7"/>
       <c r="F59" s="9"/>
       <c r="G59" s="17" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H59" s="17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I59" s="17" t="n">
         <v>29</v>
@@ -3066,10 +3045,10 @@
       <c r="E60" s="7"/>
       <c r="F60" s="9"/>
       <c r="G60" s="17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H60" s="17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I60" s="17" t="n">
         <v>30</v>
@@ -3095,10 +3074,10 @@
       <c r="E61" s="7"/>
       <c r="F61" s="9"/>
       <c r="G61" s="21" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H61" s="21" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I61" s="21" t="n">
         <v>31</v>
@@ -3122,7 +3101,7 @@
         <v>23</v>
       </c>
       <c r="C62" s="36" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D62" s="27" t="n">
         <v>46</v>
@@ -3130,10 +3109,10 @@
       <c r="E62" s="7"/>
       <c r="F62" s="9"/>
       <c r="G62" s="32" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H62" s="32" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I62" s="32" t="n">
         <v>46</v>
@@ -3157,7 +3136,7 @@
         <v>22</v>
       </c>
       <c r="C63" s="36" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D63" s="27" t="n">
         <v>47</v>
@@ -3186,7 +3165,7 @@
         <v>21</v>
       </c>
       <c r="C64" s="36" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D64" s="27" t="n">
         <v>48</v>
@@ -3215,7 +3194,7 @@
         <v>20</v>
       </c>
       <c r="C65" s="36" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D65" s="27" t="n">
         <v>49</v>
@@ -3244,7 +3223,7 @@
         <v>19</v>
       </c>
       <c r="C66" s="36" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D66" s="27" t="n">
         <v>50</v>
@@ -3273,7 +3252,7 @@
         <v>18</v>
       </c>
       <c r="C67" s="36" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D67" s="27" t="n">
         <v>51</v>
@@ -3302,7 +3281,7 @@
         <v>17</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D68" s="24" t="n">
         <v>52</v>
@@ -3331,7 +3310,7 @@
         <v>16</v>
       </c>
       <c r="C69" s="32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D69" s="24" t="n">
         <v>53</v>
@@ -3362,10 +3341,10 @@
       <c r="E70" s="7"/>
       <c r="F70" s="9"/>
       <c r="G70" s="32" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H70" s="32" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I70" s="32" t="n">
         <v>74</v>
@@ -3391,10 +3370,10 @@
       <c r="E71" s="7"/>
       <c r="F71" s="9"/>
       <c r="G71" s="32" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H71" s="32" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I71" s="32" t="n">
         <v>75</v>
@@ -3469,10 +3448,10 @@
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
       <c r="J74" s="23" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K74" s="32" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="L74" s="32" t="n">
         <v>98</v>
@@ -3500,10 +3479,10 @@
       <c r="H75" s="8"/>
       <c r="I75" s="8"/>
       <c r="J75" s="23" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K75" s="32" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="L75" s="32" t="n">
         <v>99</v>
@@ -3581,10 +3560,10 @@
       <c r="L78" s="8"/>
       <c r="M78" s="8"/>
       <c r="N78" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O78" s="32" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P78" s="33" t="n">
         <v>2</v>
@@ -3612,10 +3591,10 @@
       <c r="L79" s="8"/>
       <c r="M79" s="8"/>
       <c r="N79" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O79" s="32" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="P79" s="33" t="n">
         <v>3</v>
@@ -3636,10 +3615,10 @@
       <c r="E80" s="7"/>
       <c r="F80" s="9"/>
       <c r="G80" s="23" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H80" s="32" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I80" s="32" t="n">
         <v>24</v>
@@ -3665,10 +3644,10 @@
       <c r="E81" s="7"/>
       <c r="F81" s="9"/>
       <c r="G81" s="32" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H81" s="32" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="I81" s="32" t="n">
         <v>25</v>
@@ -3686,7 +3665,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="39" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
@@ -3709,7 +3688,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="39" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
@@ -3732,7 +3711,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="39" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B84" s="7"/>
       <c r="C84" s="8"/>
@@ -3755,7 +3734,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="39" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B85" s="7"/>
       <c r="C85" s="8"/>
@@ -3778,7 +3757,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="39" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B86" s="7"/>
       <c r="C86" s="8"/>
@@ -3801,7 +3780,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="40" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B87" s="41"/>
       <c r="C87" s="42"/>

</xml_diff>